<commit_message>
uzupełnienie bazy danych o brakujące tabele dot działu Maszyny
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Zapotrzebowanie</t>
   </si>
   <si>
-    <t>ID_operator</t>
-  </si>
-  <si>
     <t>Nazwa_dzial</t>
   </si>
   <si>
@@ -188,18 +185,9 @@
     <t>Op_imie</t>
   </si>
   <si>
-    <t>Op_masz_Maszyny</t>
-  </si>
-  <si>
     <t>ID_Op_masz_Maszyny</t>
   </si>
   <si>
-    <t>Os_zarz_Maszyny</t>
-  </si>
-  <si>
-    <t>ID_Os</t>
-  </si>
-  <si>
     <t>ID_os_zarzadzajaca</t>
   </si>
   <si>
@@ -207,6 +195,27 @@
   </si>
   <si>
     <t>Os_zarz_nazwisko</t>
+  </si>
+  <si>
+    <t>ID_propozycja</t>
+  </si>
+  <si>
+    <t>ID_stan_techniczny</t>
+  </si>
+  <si>
+    <t>ID_wykorzystanie</t>
+  </si>
+  <si>
+    <t>ID_op_maszyny</t>
+  </si>
+  <si>
+    <t>ID_Os_zarz_Maszyny</t>
+  </si>
+  <si>
+    <t>Operator_maszyny_Maszyny</t>
+  </si>
+  <si>
+    <t>Osoba_zarzadzajaca_Maszyny</t>
   </si>
 </sst>
 </file>
@@ -239,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +276,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -346,7 +373,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -357,6 +390,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF66"/>
+      <color rgb="FF66CCFF"/>
+      <color rgb="FFCC99FF"/>
       <color rgb="FFFF99CC"/>
     </mruColors>
   </colors>
@@ -671,15 +707,16 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -696,6 +733,9 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
         <v>28</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -707,6 +747,9 @@
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -718,12 +761,15 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="K4" s="4" t="s">
@@ -735,10 +781,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>35</v>
@@ -763,7 +809,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>30</v>
@@ -780,7 +826,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>30</v>
@@ -794,7 +840,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>12</v>
@@ -808,7 +854,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>40</v>
@@ -819,7 +865,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>41</v>
@@ -830,10 +876,10 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H12" t="s">
         <v>1</v>
@@ -846,11 +892,11 @@
       <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>0</v>
+      <c r="D13" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>31</v>
@@ -863,11 +909,11 @@
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>57</v>
+      <c r="D14" s="9" t="s">
+        <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>1</v>
@@ -880,8 +926,11 @@
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="D15" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="F15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -889,83 +938,101 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="H20" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="H23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Poprawiony zapis nowej pozycji w SpisForm. TODO Operator_maszyny.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -248,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -376,12 +382,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -704,335 +711,340 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
       <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="H3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="H18" t="s">
+      <c r="G18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="D19" s="15"/>
+      <c r="E19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="G20" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H23" t="s">
+      <c r="G23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="G25" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Tabela posrednia pomiędzy Maszyny a Operator_maszyny
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -714,7 +714,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,6 +836,9 @@
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Zmiana nazwy pól z Operator_maszyny na Nazwa_op_maszyny w tabeli Maszyny, Operator_maszyny_Maszyny i Operator_Maszyny
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Osoba_zarzadzajaca_Maszyny</t>
+  </si>
+  <si>
+    <t>Nazwa_op_maszyny</t>
   </si>
 </sst>
 </file>
@@ -714,7 +717,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>36</v>
@@ -837,7 +840,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>45</v>
@@ -904,7 +907,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Zmiana nazw z ID_ ... na Identyfikator klucza głównego każdej z tabel, ujednolicenie nazw kolumn w programie.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -119,15 +119,9 @@
     <t>ID_dzial</t>
   </si>
   <si>
-    <t>ID_kategoria</t>
-  </si>
-  <si>
     <t>Material</t>
   </si>
   <si>
-    <t>ID_material</t>
-  </si>
-  <si>
     <t>Nazwa_mat</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
     <t>Op_imie</t>
   </si>
   <si>
-    <t>ID_Op_masz_Maszyny</t>
-  </si>
-  <si>
     <t>ID_os_zarzadzajaca</t>
   </si>
   <si>
@@ -197,21 +188,9 @@
     <t>Os_zarz_nazwisko</t>
   </si>
   <si>
-    <t>ID_propozycja</t>
-  </si>
-  <si>
-    <t>ID_stan_techniczny</t>
-  </si>
-  <si>
-    <t>ID_wykorzystanie</t>
-  </si>
-  <si>
     <t>ID_op_maszyny</t>
   </si>
   <si>
-    <t>ID_Os_zarz_Maszyny</t>
-  </si>
-  <si>
     <t>Operator_maszyny_Maszyny</t>
   </si>
   <si>
@@ -219,6 +198,12 @@
   </si>
   <si>
     <t>Nazwa_op_maszyny</t>
+  </si>
+  <si>
+    <t>Nazwa_os_zarzadzajaca</t>
+  </si>
+  <si>
+    <t>Identyfikator</t>
   </si>
 </sst>
 </file>
@@ -717,7 +702,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +711,7 @@
     <col min="2" max="2" width="3.7109375" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="4.28515625" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -739,12 +724,12 @@
         <v>27</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -753,7 +738,7 @@
         <v>28</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -767,7 +752,7 @@
         <v>29</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -775,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>20</v>
@@ -795,13 +780,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -812,10 +797,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -823,7 +808,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>30</v>
@@ -832,24 +817,21 @@
         <v>12</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -857,13 +839,13 @@
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -871,10 +853,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -882,44 +864,44 @@
         <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -930,13 +912,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>1</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -944,10 +926,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -977,10 +959,10 @@
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -988,7 +970,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>19</v>
@@ -1007,7 +989,7 @@
         <v>19</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1015,7 +997,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G23" t="s">
         <v>18</v>
@@ -1026,10 +1008,10 @@
         <v>22</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ID maszyn dla wybranego operatora, dodanie przycisków do wgrania zdjęcia do tabeli Maszyny
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Producent</t>
   </si>
   <si>
-    <t>Zdjecie1</t>
-  </si>
-  <si>
-    <t>Rozszerz_zdj1</t>
-  </si>
-  <si>
     <t>Osoba_zarzadzajaca</t>
   </si>
   <si>
@@ -204,6 +198,15 @@
   </si>
   <si>
     <t>Identyfikator</t>
+  </si>
+  <si>
+    <t>Zdjecie</t>
+  </si>
+  <si>
+    <t>Rozszerz_zdj</t>
+  </si>
+  <si>
+    <t>Zawartosc_pliku</t>
   </si>
 </sst>
 </file>
@@ -699,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,24 +724,24 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -746,13 +749,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -760,16 +763,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>3</v>
@@ -780,13 +783,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -797,10 +800,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -808,16 +811,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -825,13 +828,13 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -839,202 +842,207 @@
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>58</v>
+      <c r="A12" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
+      <c r="A14" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>1</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>12</v>
+      <c r="A15" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>13</v>
+      <c r="A16" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
-        <v>18</v>
+      <c r="A21" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>19</v>
+      <c r="A22" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>21</v>
+      <c r="A23" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
interfejs materiały - wstępny szkic
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -122,18 +122,9 @@
     <t>Rodzaj</t>
   </si>
   <si>
-    <t>Ilosc</t>
-  </si>
-  <si>
     <t>Wart_jedn</t>
   </si>
   <si>
-    <t>Dostawca1</t>
-  </si>
-  <si>
-    <t>Dostawca2</t>
-  </si>
-  <si>
     <t>Stan_magazynowy</t>
   </si>
   <si>
@@ -207,6 +198,15 @@
   </si>
   <si>
     <t>Zawartosc_pliku</t>
+  </si>
+  <si>
+    <t>Dostawca</t>
+  </si>
+  <si>
+    <t>Link_dostawca</t>
+  </si>
+  <si>
+    <t>Dod_info_dostawca</t>
   </si>
 </sst>
 </file>
@@ -239,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +291,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -380,6 +392,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -702,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,9 +738,10 @@
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -730,9 +749,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
@@ -740,16 +759,16 @@
       <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>27</v>
@@ -757,13 +776,16 @@
       <c r="J3" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>18</v>
@@ -774,25 +796,31 @@
       <c r="H4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -800,18 +828,21 @@
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>28</v>
@@ -819,125 +850,140 @@
       <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="J9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="3" t="s">
+      <c r="L10" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>10</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -962,10 +1008,10 @@
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -973,7 +1019,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>17</v>
@@ -992,7 +1038,7 @@
         <v>16</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1000,7 +1046,7 @@
         <v>17</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G23" t="s">
         <v>16</v>
@@ -1011,10 +1057,10 @@
         <v>19</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
uzupełnienie dokumentacji dot materiałów
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -207,6 +207,24 @@
   </si>
   <si>
     <t>Dod_info_dostawca</t>
+  </si>
+  <si>
+    <t>Stan_magazynowy_po</t>
+  </si>
+  <si>
+    <t>Nazwa_dostawca</t>
+  </si>
+  <si>
+    <t>Nazwa_rodzaj</t>
+  </si>
+  <si>
+    <t>Dostawca_Material</t>
+  </si>
+  <si>
+    <t>ID_material</t>
+  </si>
+  <si>
+    <t>ID_dostawca</t>
   </si>
 </sst>
 </file>
@@ -239,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +321,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -396,6 +420,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -720,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,11 +770,12 @@
     <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -749,7 +783,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -763,7 +797,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -777,10 +811,13 @@
         <v>30</v>
       </c>
       <c r="L3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -796,14 +833,17 @@
       <c r="H4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -813,14 +853,17 @@
       <c r="E5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -833,11 +876,14 @@
       <c r="J6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -850,14 +896,14 @@
       <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -871,7 +917,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -882,13 +928,13 @@
         <v>10</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="N9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>55</v>
       </c>
@@ -896,13 +942,13 @@
         <v>40</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
@@ -910,13 +956,13 @@
         <v>41</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>56</v>
       </c>
@@ -933,7 +979,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>53</v>
       </c>
@@ -946,8 +992,11 @@
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>52</v>
       </c>
@@ -960,11 +1009,11 @@
       <c r="G14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -974,15 +1023,15 @@
       <c r="E15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="N16" s="17" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
wstępny szkic interfejsu Normalia + dokumentacja
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -225,6 +225,27 @@
   </si>
   <si>
     <t>ID_dostawca</t>
+  </si>
+  <si>
+    <t>Normalia</t>
+  </si>
+  <si>
+    <t>Dostawca_normaliow</t>
+  </si>
+  <si>
+    <t>Nazwa_dostawca_normaliow</t>
+  </si>
+  <si>
+    <t>Nazwa_nor</t>
+  </si>
+  <si>
+    <t>Typ_nor</t>
+  </si>
+  <si>
+    <t>Rodzaj_nor</t>
+  </si>
+  <si>
+    <t>Wart_jedn_nor</t>
   </si>
 </sst>
 </file>
@@ -257,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,6 +348,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -429,6 +462,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -753,37 +792,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" customWidth="1"/>
     <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.28515625" customWidth="1"/>
+    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.5703125" customWidth="1"/>
+    <col min="18" max="18" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -796,8 +844,11 @@
       <c r="J2" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -816,8 +867,14 @@
       <c r="N3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -842,8 +899,14 @@
       <c r="N4" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -862,8 +925,14 @@
       <c r="N5" s="19" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P5" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -882,8 +951,14 @@
       <c r="N6" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -902,8 +977,14 @@
       <c r="N7" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P7" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -916,8 +997,11 @@
       <c r="J8" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P8" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -933,8 +1017,11 @@
       <c r="N9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>55</v>
       </c>
@@ -947,8 +1034,11 @@
       <c r="N10" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P10" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
@@ -961,8 +1051,11 @@
       <c r="N11" s="16" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>56</v>
       </c>
@@ -978,8 +1071,11 @@
       <c r="J12" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>53</v>
       </c>
@@ -995,8 +1091,11 @@
       <c r="J13" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P13" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>52</v>
       </c>
@@ -1013,7 +1112,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1027,7 +1126,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Uzupełnienie bazy danych o tabelę Materiał i Normalia
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -104,12 +104,6 @@
     <t>Maszyny</t>
   </si>
   <si>
-    <t>Czestotliwosc</t>
-  </si>
-  <si>
-    <t>ID_czestotliwosc</t>
-  </si>
-  <si>
     <t>ID_dzial</t>
   </si>
   <si>
@@ -119,27 +113,6 @@
     <t>Nazwa_mat</t>
   </si>
   <si>
-    <t>Rodzaj</t>
-  </si>
-  <si>
-    <t>Wart_jedn</t>
-  </si>
-  <si>
-    <t>Stan_magazynowy</t>
-  </si>
-  <si>
-    <t>Stan_min</t>
-  </si>
-  <si>
-    <t>Zuzycie</t>
-  </si>
-  <si>
-    <t>Odpad</t>
-  </si>
-  <si>
-    <t>Zapotrzebowanie</t>
-  </si>
-  <si>
     <t>Nazwa_dzial</t>
   </si>
   <si>
@@ -200,52 +173,118 @@
     <t>Zawartosc_pliku</t>
   </si>
   <si>
-    <t>Dostawca</t>
-  </si>
-  <si>
-    <t>Link_dostawca</t>
-  </si>
-  <si>
-    <t>Dod_info_dostawca</t>
-  </si>
-  <si>
-    <t>Stan_magazynowy_po</t>
-  </si>
-  <si>
-    <t>Nazwa_dostawca</t>
-  </si>
-  <si>
-    <t>Nazwa_rodzaj</t>
-  </si>
-  <si>
     <t>Dostawca_Material</t>
   </si>
   <si>
     <t>ID_material</t>
   </si>
   <si>
-    <t>ID_dostawca</t>
-  </si>
-  <si>
     <t>Normalia</t>
   </si>
   <si>
-    <t>Dostawca_normaliow</t>
-  </si>
-  <si>
-    <t>Nazwa_dostawca_normaliow</t>
-  </si>
-  <si>
-    <t>Nazwa_nor</t>
-  </si>
-  <si>
-    <t>Typ_nor</t>
-  </si>
-  <si>
-    <t>Rodzaj_nor</t>
-  </si>
-  <si>
-    <t>Wart_jedn_nor</t>
+    <t>Stan_mat</t>
+  </si>
+  <si>
+    <t>Typ_mat</t>
+  </si>
+  <si>
+    <t>Rodzaj_mat</t>
+  </si>
+  <si>
+    <t>Zuzycie_mat</t>
+  </si>
+  <si>
+    <t>Odpad_mat</t>
+  </si>
+  <si>
+    <t>Stan_min_mat</t>
+  </si>
+  <si>
+    <t>Zapotrzebowanie_mat</t>
+  </si>
+  <si>
+    <t>Stan_mag_po_mat</t>
+  </si>
+  <si>
+    <t>Dostawca_mat</t>
+  </si>
+  <si>
+    <t>Nazwa_dostawca_mat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Nazwa_dostawca_norm</t>
+  </si>
+  <si>
+    <t>Link_dostawca_norm</t>
+  </si>
+  <si>
+    <t>Dod_info_dostawca_norm</t>
+  </si>
+  <si>
+    <t>Dod_info_dostawca_mat</t>
+  </si>
+  <si>
+    <t>Link_dostawca_mat</t>
+  </si>
+  <si>
+    <t>Jednostka_miar</t>
+  </si>
+  <si>
+    <t>Nazwa_jednostka_miar</t>
+  </si>
+  <si>
+    <t>Nazwa_norm</t>
+  </si>
+  <si>
+    <t>Typ_norm</t>
+  </si>
+  <si>
+    <t>Rodzaj_norm</t>
+  </si>
+  <si>
+    <t>Dostawca_norm</t>
+  </si>
+  <si>
+    <t>Stan_norm</t>
+  </si>
+  <si>
+    <t>Zuzycie_norm</t>
+  </si>
+  <si>
+    <t>Odpad_norm</t>
+  </si>
+  <si>
+    <t>Stan_min_norm</t>
+  </si>
+  <si>
+    <t>Zapotrzebowanie_norm</t>
+  </si>
+  <si>
+    <t>Stan_mag_po_norm</t>
+  </si>
+  <si>
+    <t>Dostawca_Normalia</t>
+  </si>
+  <si>
+    <t>ID_normalia</t>
+  </si>
+  <si>
+    <t>ID_dostawca_mat</t>
+  </si>
+  <si>
+    <t>ID_dostawca_norm</t>
+  </si>
+  <si>
+    <t>Nazwa_rodzaj_mat</t>
+  </si>
+  <si>
+    <t>Jednostka_miar_mat</t>
+  </si>
+  <si>
+    <t>Jednostka_miar_norm</t>
   </si>
 </sst>
 </file>
@@ -278,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,12 +356,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF66CCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -335,18 +368,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -359,7 +380,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,32 +475,34 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -478,6 +513,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF6600"/>
       <color rgb="FF99FF66"/>
       <color rgb="FF66CCFF"/>
       <color rgb="FFCC99FF"/>
@@ -792,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,81 +841,79 @@
     <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.28515625" customWidth="1"/>
     <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="3.140625" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.28515625" customWidth="1"/>
-    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.5703125" customWidth="1"/>
-    <col min="18" max="18" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5703125" customWidth="1"/>
+    <col min="17" max="17" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5703125" customWidth="1"/>
+    <col min="19" max="19" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" t="s">
-        <v>58</v>
-      </c>
-      <c r="P3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="R3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q3" t="s">
+        <v>80</v>
+      </c>
+      <c r="S3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>18</v>
@@ -887,52 +921,55 @@
       <c r="G4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" s="18" t="s">
+      <c r="I4" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="P5" s="21" t="s">
+      <c r="K5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="O5" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="R5" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q5" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="S5" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -940,206 +977,209 @@
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P6" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="N7" s="3" t="s">
+      <c r="I7" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="P7" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="I9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="N14" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N16" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1150,68 +1190,70 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="15"/>
       <c r="E19" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="I21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>20</v>
       </c>
@@ -1219,22 +1261,22 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
wymiana danych z tabelą Materiały Access2DB
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Access komunikacja z tabelą Dostawca_mat, uporządzkowanie kodu, poprawki w Access2DB.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>Jednostka_miar_norm</t>
+  </si>
+  <si>
+    <t>ID_</t>
   </si>
 </sst>
 </file>
@@ -830,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
@@ -1174,12 +1177,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>15</v>
       </c>
@@ -1223,7 +1226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>16</v>
       </c>
@@ -1231,7 +1234,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>17</v>
       </c>
@@ -1241,8 +1244,11 @@
       <c r="G23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>19</v>
       </c>
@@ -1253,7 +1259,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>20</v>
       </c>
@@ -1261,22 +1267,22 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Zmiana słowników operator_maszyny na check-boxy umozliwiające zaznaczenie kilku operatorów dla 1 maszyny.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
poprawki w check-box operator maszyny tabela maszyny.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -853,25 +853,25 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="1.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="1.5703125" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3" customWidth="1"/>
+    <col min="6" max="6" width="1.140625" customWidth="1"/>
     <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" customWidth="1"/>
+    <col min="8" max="8" width="1.42578125" customWidth="1"/>
     <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="10" width="3.140625" customWidth="1"/>
+    <col min="10" max="10" width="1" customWidth="1"/>
     <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" customWidth="1"/>
+    <col min="12" max="12" width="1.140625" customWidth="1"/>
     <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.140625" customWidth="1"/>
+    <col min="14" max="14" width="1.28515625" customWidth="1"/>
     <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="16" max="16" width="1.28515625" customWidth="1"/>
     <col min="17" max="17" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.5703125" customWidth="1"/>
+    <col min="18" max="18" width="1.140625" customWidth="1"/>
     <col min="19" max="19" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.5703125" customWidth="1"/>
+    <col min="20" max="20" width="1" customWidth="1"/>
     <col min="21" max="21" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Poprawienie wyświetlania się operatorów po zmianie indeksu zakładek. Dezaktywaja okna maszyn operatora i jego odświeżania po zmianie indeksu operatora.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RemaGUM\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8023A43B-6F21-4776-945D-B0A69505882E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2B79A03-1346-4E39-9243-8DD340F5CD22}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -102,13 +102,7 @@
     <t>Maszyny</t>
   </si>
   <si>
-    <t>ID_dzial</t>
-  </si>
-  <si>
     <t>Nazwa_mat</t>
-  </si>
-  <si>
-    <t>Nazwa_dzial</t>
   </si>
   <si>
     <t>Uprawnienie</t>
@@ -450,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -480,9 +474,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -848,7 +839,7 @@
   <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,19 +867,19 @@
     <col min="21" max="21" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="E1" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" s="24" t="s">
-        <v>84</v>
+    <row r="1" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="E1" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -896,54 +887,54 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="S2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="U2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -957,63 +948,63 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="U4" s="20" t="s">
         <v>57</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="S4" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="U4" s="21" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>49</v>
+        <v>36</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="S5" s="22" t="s">
-        <v>79</v>
+        <v>61</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" s="21" t="s">
+        <v>77</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1024,22 +1015,22 @@
         <v>3</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>46</v>
+        <v>26</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q6" s="18" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="Q6" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1047,16 +1038,16 @@
         <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q7" s="19" t="s">
-        <v>82</v>
+        <v>27</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1064,33 +1055,33 @@
         <v>5</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q8" s="21" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="20" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>30</v>
+      <c r="G9" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1098,36 +1089,36 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>65</v>
+        <v>37</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1135,39 +1126,36 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E13" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1175,13 +1163,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1205,29 +1193,29 @@
         <v>11</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>25</v>
+      <c r="G19" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1235,41 +1223,38 @@
         <v>14</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="K22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -1296,14 +1281,14 @@
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="5" t="s">

</xml_diff>

<commit_message>
Poprawki i porządkowanie kodu.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RemaGUM\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2B79A03-1346-4E39-9243-8DD340F5CD22}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{891D22F8-A291-443F-B03E-2B330191493B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="86">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>Operator</t>
-  </si>
-  <si>
-    <t>Nazwa_operatora</t>
   </si>
   <si>
     <t>Maszyny_Operator</t>
@@ -839,7 +836,7 @@
   <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G4" sqref="G4:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +884,7 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>84</v>
@@ -947,8 +944,8 @@
       <c r="E4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>85</v>
+      <c r="G4" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>39</v>
@@ -982,8 +979,8 @@
       <c r="E5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>10</v>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>78</v>
@@ -1015,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K6" s="19" t="s">
         <v>48</v>
@@ -1038,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>79</v>
@@ -1054,8 +1051,8 @@
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>28</v>
+      <c r="G8" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="I8" t="s">
         <v>62</v>
@@ -1071,8 +1068,8 @@
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>29</v>
+      <c r="G9" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>39</v>
@@ -1092,7 +1089,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>63</v>
@@ -1112,7 +1109,7 @@
         <v>39</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>50</v>
@@ -1130,9 +1127,6 @@
       </c>
       <c r="E12" s="9" t="s">
         <v>0</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Poprawa indeksów operatora przy dodaniu nowego operatora.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RemaGUM\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{891D22F8-A291-443F-B03E-2B330191493B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A7FE8BBE-2639-4794-8458-8DBA24671BD5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -836,7 +836,7 @@
   <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Poprawki listy sortowania operatorów.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RemaGUM\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A7FE8BBE-2639-4794-8458-8DBA24671BD5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{756B7836-EE47-46B5-9608-65EEB0860483}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ustalenie powiązań kluczy między tabelami w bazie Access.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RemaGUM\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{756B7836-EE47-46B5-9608-65EEB0860483}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F4F7F4EF-DC65-4D71-A5C2-1A9BABCC7BD0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Producent</t>
   </si>
   <si>
-    <t>Osoba_zarzadzajaca</t>
-  </si>
-  <si>
     <t>Nr_pom</t>
   </si>
   <si>
@@ -126,24 +123,9 @@
     <t>Op_imie</t>
   </si>
   <si>
-    <t>ID_os_zarzadzajaca</t>
-  </si>
-  <si>
-    <t>Os_zarz_imie</t>
-  </si>
-  <si>
-    <t>Os_zarz_nazwisko</t>
-  </si>
-  <si>
     <t>ID_op_maszyny</t>
   </si>
   <si>
-    <t>Osoba_zarzadzajaca_Maszyny</t>
-  </si>
-  <si>
-    <t>Nazwa_os_zarzadzajaca</t>
-  </si>
-  <si>
     <t>Identyfikator</t>
   </si>
   <si>
@@ -283,6 +265,33 @@
   </si>
   <si>
     <t>Maszyny_Operator</t>
+  </si>
+  <si>
+    <t>ID_dysponent</t>
+  </si>
+  <si>
+    <t>Maszyny_Dysponent</t>
+  </si>
+  <si>
+    <t>Maszyny_nazwa</t>
+  </si>
+  <si>
+    <t>Nazwa_dysponent</t>
+  </si>
+  <si>
+    <t>Dysp_nazwisko</t>
+  </si>
+  <si>
+    <t>Dysp_imie</t>
+  </si>
+  <si>
+    <t>Dysp_dane</t>
+  </si>
+  <si>
+    <t>Dysponent</t>
+  </si>
+  <si>
+    <t>Maszyny_nazwa_Dysp</t>
   </si>
 </sst>
 </file>
@@ -835,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,77 +875,77 @@
   <sheetData>
     <row r="1" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C1" s="22"/>
       <c r="E1" s="23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="M1" s="23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="O2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="Q2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="S2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="U2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>1</v>
@@ -945,89 +954,92 @@
         <v>0</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="S4" s="20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="U4" s="20" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="S5" s="21" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="G6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="O6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q6" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="Q6" s="17" t="s">
-        <v>66</v>
-      </c>
       <c r="U6" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1035,16 +1047,16 @@
         <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1052,16 +1064,16 @@
         <v>5</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1069,16 +1081,16 @@
         <v>6</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1086,36 +1098,36 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>31</v>
+        <v>81</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="I10" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q10" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1123,33 +1135,33 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>0</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1157,136 +1169,139 @@
         <v>1</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>38</v>
+        <v>83</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>35</v>
+        <v>13</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodatkowe pole w BD Magazyn, usunięcie z DB normaliów, dodanie w Access2DB obsługi Magazynu (SQL), obsługa danych słownikowych Magazynu.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RemaGUM\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F63C8210-EF66-4000-85F3-878258E4C957}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{341F274D-4CF3-4511-9978-E65482F609DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -144,9 +144,6 @@
     <t>ID_material</t>
   </si>
   <si>
-    <t>Normalia</t>
-  </si>
-  <si>
     <t>Stan_mat</t>
   </si>
   <si>
@@ -180,15 +177,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Nazwa_dostawca_norm</t>
-  </si>
-  <si>
-    <t>Link_dostawca_norm</t>
-  </si>
-  <si>
-    <t>Dod_info_dostawca_norm</t>
-  </si>
-  <si>
     <t>Dod_info_dostawca_mat</t>
   </si>
   <si>
@@ -201,57 +189,15 @@
     <t>Nazwa_jednostka_miar</t>
   </si>
   <si>
-    <t>Nazwa_norm</t>
-  </si>
-  <si>
-    <t>Typ_norm</t>
-  </si>
-  <si>
-    <t>Rodzaj_norm</t>
-  </si>
-  <si>
-    <t>Dostawca_norm</t>
-  </si>
-  <si>
-    <t>Stan_norm</t>
-  </si>
-  <si>
-    <t>Zuzycie_norm</t>
-  </si>
-  <si>
-    <t>Odpad_norm</t>
-  </si>
-  <si>
-    <t>Stan_min_norm</t>
-  </si>
-  <si>
-    <t>Zapotrzebowanie_norm</t>
-  </si>
-  <si>
-    <t>Stan_mag_po_norm</t>
-  </si>
-  <si>
-    <t>Dostawca_Normalia</t>
-  </si>
-  <si>
-    <t>ID_normalia</t>
-  </si>
-  <si>
     <t>ID_dostawca_mat</t>
   </si>
   <si>
-    <t>ID_dostawca_norm</t>
-  </si>
-  <si>
     <t>Nazwa_rodzaj_mat</t>
   </si>
   <si>
     <t>Jednostka_miar_mat</t>
   </si>
   <si>
-    <t>Jednostka_miar_norm</t>
-  </si>
-  <si>
     <t>SŁOWNIKI</t>
   </si>
   <si>
@@ -295,6 +241,12 @@
   </si>
   <si>
     <t>Maszyny_nazwa_D</t>
+  </si>
+  <si>
+    <t>Magazyn</t>
+  </si>
+  <si>
+    <t>Wybor_magazynu</t>
   </si>
 </sst>
 </file>
@@ -327,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,12 +336,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -402,13 +348,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -509,19 +455,13 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -845,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,56 +808,41 @@
     <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="1.28515625" customWidth="1"/>
     <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="1.28515625" customWidth="1"/>
-    <col min="17" max="17" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="1.140625" customWidth="1"/>
-    <col min="19" max="19" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="1" customWidth="1"/>
-    <col min="21" max="21" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="E1" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="E1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="O2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" t="s">
-        <v>68</v>
-      </c>
-      <c r="U2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
@@ -928,7 +853,7 @@
         <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>33</v>
@@ -936,17 +861,8 @@
       <c r="O3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -969,19 +885,10 @@
         <v>37</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="S4" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="U4" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -994,29 +901,20 @@
       <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="19" t="s">
-        <v>72</v>
+      <c r="I5" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="S5" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1024,45 +922,36 @@
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="19" t="s">
-        <v>42</v>
+      <c r="K6" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="M6" s="15" t="s">
         <v>38</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q6" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="18" t="s">
-        <v>73</v>
+      <c r="K7" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q7" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1070,16 +959,13 @@
         <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q8" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1090,33 +976,30 @@
         <v>33</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="18" t="s">
-        <v>57</v>
+      <c r="I10" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="M10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1127,13 +1010,13 @@
         <v>31</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1144,13 +1027,13 @@
         <v>0</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1158,43 +1041,40 @@
         <v>35</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1216,7 +1096,7 @@
         <v>11</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1227,7 +1107,7 @@
         <v>12</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1243,7 +1123,7 @@
         <v>14</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1254,10 +1134,10 @@
         <v>15</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="K22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Zaprojektowanie i dodanie nowych tabel do bazy danych dot lab. chemii - propozycja.
</commit_message>
<xml_diff>
--- a/Docs/Projekt BD.xlsx
+++ b/Docs/Projekt BD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RemaGUM\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{09EF9190-F1FC-4740-A259-F2136C6BBAB0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03731E99-02DD-42C9-B5A9-6AAD847154AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="97">
   <si>
     <t>ID_maszyny</t>
   </si>
@@ -247,6 +247,75 @@
   </si>
   <si>
     <t>Wybor_magazynu</t>
+  </si>
+  <si>
+    <t>Przyrzad</t>
+  </si>
+  <si>
+    <t>Nazwa_przyrzadu</t>
+  </si>
+  <si>
+    <t>Typ_przyrzadu</t>
+  </si>
+  <si>
+    <t>Rodzaj_przyrzadu</t>
+  </si>
+  <si>
+    <t>Nr_fabryczny_przyrzadu</t>
+  </si>
+  <si>
+    <t>Nr_systemowy_przyrzadu</t>
+  </si>
+  <si>
+    <t>Dane_producenta_przyrzadu</t>
+  </si>
+  <si>
+    <t>Data_ost_przegl_przyrzadu</t>
+  </si>
+  <si>
+    <t>Opiekun_przyrzadu</t>
+  </si>
+  <si>
+    <t>Zdjecie_przyrzadu</t>
+  </si>
+  <si>
+    <t>Zawartosc_pliku_zdj_przyrzadu</t>
+  </si>
+  <si>
+    <t>Rozszerz_zdj_przyrzadu</t>
+  </si>
+  <si>
+    <t>Rok_ost_przeg_przyrzadu</t>
+  </si>
+  <si>
+    <t>Mc_ost_przeg_przyrzadu</t>
+  </si>
+  <si>
+    <t>Dz_ost_przeg_przyrzadu</t>
+  </si>
+  <si>
+    <t>Imie_opiekuna</t>
+  </si>
+  <si>
+    <t>Nazwisko_opiekuna</t>
+  </si>
+  <si>
+    <t>Dzial_opiekuna</t>
+  </si>
+  <si>
+    <t>Dane_dodatkowe_opiekuna</t>
+  </si>
+  <si>
+    <t>Stanowisko</t>
+  </si>
+  <si>
+    <t>Przyrzady_na_stanowisku</t>
+  </si>
+  <si>
+    <t>Dane_stanowiska</t>
+  </si>
+  <si>
+    <t>Nazwa_stanowiska</t>
   </si>
 </sst>
 </file>
@@ -279,7 +348,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +424,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6600FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -462,6 +549,15 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -469,7 +565,76 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
+      <color rgb="FF6600FF"/>
+      <color rgb="FFFF9900"/>
+      <color rgb="FFCC66FF"/>
       <color rgb="FFFF6600"/>
       <color rgb="FF99FF66"/>
       <color rgb="FF66CCFF"/>
@@ -496,7 +661,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CFC7A9"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -785,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,9 +973,13 @@
     <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="1.28515625" customWidth="1"/>
     <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="1.42578125" customWidth="1"/>
+    <col min="17" max="17" width="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="1.7109375" customWidth="1"/>
+    <col min="19" max="19" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>57</v>
       </c>
@@ -825,7 +994,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
@@ -841,8 +1010,15 @@
       <c r="O2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="22"/>
+      <c r="Q2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
@@ -861,8 +1037,15 @@
       <c r="O3" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="22"/>
+      <c r="Q3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -887,8 +1070,15 @@
       <c r="O4" s="15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="22"/>
+      <c r="Q4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -913,8 +1103,15 @@
       <c r="O5" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P5" s="22"/>
+      <c r="Q5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -936,8 +1133,15 @@
       <c r="O6" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="22"/>
+      <c r="Q6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -950,8 +1154,15 @@
       <c r="M7" s="16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P7" s="22"/>
+      <c r="Q7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
@@ -964,8 +1175,12 @@
       <c r="K8" s="15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P8" s="22"/>
+      <c r="Q8" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
@@ -978,8 +1193,12 @@
       <c r="K9" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P9" s="22"/>
+      <c r="Q9" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
@@ -998,8 +1217,12 @@
       <c r="M10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P10" s="22"/>
+      <c r="Q10" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1015,8 +1238,15 @@
       <c r="M11" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P11" s="22"/>
+      <c r="Q11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="S11" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1032,8 +1262,15 @@
       <c r="M12" s="21" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="22"/>
+      <c r="Q12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1046,8 +1283,15 @@
       <c r="K13" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P13" s="22"/>
+      <c r="Q13" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>1</v>
       </c>
@@ -1060,24 +1304,42 @@
       <c r="K14" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P14" s="22"/>
+      <c r="Q14" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P15" s="22"/>
+      <c r="Q15" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G16" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P16" s="22"/>
+      <c r="Q16" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1087,8 +1349,12 @@
       <c r="G17" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P17" s="22"/>
+      <c r="Q17" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1098,8 +1364,12 @@
       <c r="G18" s="9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P18" s="22"/>
+      <c r="Q18" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>14</v>
       </c>
@@ -1109,16 +1379,18 @@
       <c r="G19" s="9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P19" s="22"/>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P20" s="22"/>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="13" t="s">
         <v>14</v>
       </c>
@@ -1126,7 +1398,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1140,7 +1412,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1148,7 +1420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>15</v>
       </c>
@@ -1156,17 +1428,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1174,7 +1446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -1182,7 +1454,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>16</v>
       </c>

</xml_diff>